<commit_message>
Update V1.2_新增字段_修订中和Java对比 - Copy.xlsx
</commit_message>
<xml_diff>
--- a/work/V1.2_新增字段_修订中和Java对比 - Copy.xlsx
+++ b/work/V1.2_新增字段_修订中和Java对比 - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caianhua\Documents\GitHub\hillcat.github.io\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB544888-47F3-4081-A5E6-A852EACA8BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF4748D-4560-43E3-AD63-93277F4006D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="1320" windowWidth="21630" windowHeight="15090" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="新增字段" sheetId="1" r:id="rId1"/>
@@ -174,7 +174,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="B400" authorId="0" shapeId="0" xr:uid="{C32D8B73-0C8C-4F65-8274-0B7FB4A24F07}">
+    <comment ref="D388" authorId="1" shapeId="0" xr:uid="{8AF632A3-371F-4F83-86D3-073AF4779489}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>前端对接的时候发现后端漏掉了这个字段，后来才加上。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B401" authorId="0" shapeId="0" xr:uid="{C32D8B73-0C8C-4F65-8274-0B7FB4A24F07}">
       <text>
         <r>
           <rPr>
@@ -188,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B429" authorId="0" shapeId="0" xr:uid="{C7010E88-7161-4797-8E10-9960E146B4C0}">
+    <comment ref="B430" authorId="0" shapeId="0" xr:uid="{C7010E88-7161-4797-8E10-9960E146B4C0}">
       <text>
         <r>
           <rPr>
@@ -202,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B453" authorId="0" shapeId="0" xr:uid="{5D0E2CB7-D5FB-4E80-8F1E-D5A555A8DF66}">
+    <comment ref="B454" authorId="0" shapeId="0" xr:uid="{5D0E2CB7-D5FB-4E80-8F1E-D5A555A8DF66}">
       <text>
         <r>
           <rPr>
@@ -216,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C454" authorId="1" shapeId="0" xr:uid="{26593D68-268D-4A9E-AF8E-94121472E8BA}">
+    <comment ref="C455" authorId="1" shapeId="0" xr:uid="{26593D68-268D-4A9E-AF8E-94121472E8BA}">
       <text>
         <r>
           <rPr>
@@ -231,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B477" authorId="0" shapeId="0" xr:uid="{CE2A2A41-47D2-4215-8548-D04DE9D77AA2}">
+    <comment ref="B478" authorId="0" shapeId="0" xr:uid="{CE2A2A41-47D2-4215-8548-D04DE9D77AA2}">
       <text>
         <r>
           <rPr>
@@ -255,12 +270,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="D488" authorId="1" shapeId="0" xr:uid="{15B197AC-29AA-4B87-9C50-3BBA85874A67}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>前端对接时候发现后端没有这个字段。</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2948" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="934">
   <si>
     <t>字段名</t>
   </si>
@@ -3876,6 +3917,26 @@
   </si>
   <si>
     <t>top_girder_width</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">桥面板截面形式 </t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>stiffening_beam_type</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>cable_saddle_form</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>索鞍形式</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>加劲梁类型</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -4721,11 +4782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H647"/>
+  <dimension ref="A1:H650"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A632" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B654" sqref="B654"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11153,20 +11214,14 @@
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A388" t="s">
-        <v>650</v>
-      </c>
       <c r="B388" t="s">
         <v>701</v>
       </c>
-      <c r="C388" t="s">
-        <v>526</v>
-      </c>
-      <c r="D388" t="s">
-        <v>512</v>
-      </c>
-      <c r="G388" t="s">
-        <v>28</v>
+      <c r="C388" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="D388" s="4" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.2">
@@ -11176,11 +11231,14 @@
       <c r="B389" t="s">
         <v>701</v>
       </c>
-      <c r="C389" s="33" t="s">
-        <v>917</v>
-      </c>
-      <c r="D389" s="53" t="s">
-        <v>667</v>
+      <c r="C389" t="s">
+        <v>526</v>
+      </c>
+      <c r="D389" t="s">
+        <v>512</v>
+      </c>
+      <c r="G389" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.2">
@@ -11191,10 +11249,10 @@
         <v>701</v>
       </c>
       <c r="C390" s="33" t="s">
-        <v>678</v>
+        <v>917</v>
       </c>
       <c r="D390" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="391" spans="1:7" x14ac:dyDescent="0.2">
@@ -11205,10 +11263,10 @@
         <v>701</v>
       </c>
       <c r="C391" s="33" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D391" s="53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.2">
@@ -11219,10 +11277,10 @@
         <v>701</v>
       </c>
       <c r="C392" s="33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D392" s="53" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="393" spans="1:7" x14ac:dyDescent="0.2">
@@ -11233,10 +11291,10 @@
         <v>701</v>
       </c>
       <c r="C393" s="33" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D393" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.2">
@@ -11247,10 +11305,10 @@
         <v>701</v>
       </c>
       <c r="C394" s="33" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="D394" s="53" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.2">
@@ -11261,10 +11319,10 @@
         <v>701</v>
       </c>
       <c r="C395" s="33" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D395" s="53" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.2">
@@ -11275,10 +11333,10 @@
         <v>701</v>
       </c>
       <c r="C396" s="33" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D396" s="53" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="397" spans="1:7" x14ac:dyDescent="0.2">
@@ -11289,10 +11347,10 @@
         <v>701</v>
       </c>
       <c r="C397" s="33" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D397" s="53" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.2">
@@ -11303,38 +11361,38 @@
         <v>701</v>
       </c>
       <c r="C398" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="D398" s="53" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
+        <v>650</v>
+      </c>
+      <c r="B399" t="s">
+        <v>701</v>
+      </c>
+      <c r="C399" s="33" t="s">
         <v>685</v>
       </c>
-      <c r="D398" s="53" t="s">
+      <c r="D399" s="53" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A400" s="4" t="s">
+    <row r="401" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A401" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="B400" s="23" t="s">
+      <c r="B401" s="23" t="s">
         <v>913</v>
       </c>
-      <c r="C400" t="s">
+      <c r="C401" t="s">
         <v>60</v>
       </c>
-      <c r="D400" t="s">
+      <c r="D401" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="401" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A401" t="s">
-        <v>651</v>
-      </c>
-      <c r="B401" t="s">
-        <v>702</v>
-      </c>
-      <c r="C401" t="s">
-        <v>534</v>
-      </c>
-      <c r="D401" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.2">
@@ -11344,14 +11402,11 @@
       <c r="B402" t="s">
         <v>702</v>
       </c>
-      <c r="C402" s="4" t="s">
-        <v>536</v>
+      <c r="C402" t="s">
+        <v>534</v>
       </c>
       <c r="D402" t="s">
-        <v>535</v>
-      </c>
-      <c r="G402" t="s">
-        <v>28</v>
+        <v>533</v>
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.2">
@@ -11361,11 +11416,11 @@
       <c r="B403" t="s">
         <v>702</v>
       </c>
-      <c r="C403" t="s">
-        <v>537</v>
+      <c r="C403" s="4" t="s">
+        <v>536</v>
       </c>
       <c r="D403" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="G403" t="s">
         <v>28</v>
@@ -11379,10 +11434,10 @@
         <v>702</v>
       </c>
       <c r="C404" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D404" t="s">
-        <v>657</v>
+        <v>528</v>
       </c>
       <c r="G404" t="s">
         <v>28</v>
@@ -11395,11 +11450,11 @@
       <c r="B405" t="s">
         <v>702</v>
       </c>
-      <c r="C405" s="4" t="s">
-        <v>459</v>
+      <c r="C405" t="s">
+        <v>540</v>
       </c>
       <c r="D405" t="s">
-        <v>546</v>
+        <v>657</v>
       </c>
       <c r="G405" t="s">
         <v>28</v>
@@ -11412,11 +11467,11 @@
       <c r="B406" t="s">
         <v>702</v>
       </c>
-      <c r="C406" t="s">
-        <v>526</v>
+      <c r="C406" s="4" t="s">
+        <v>459</v>
       </c>
       <c r="D406" t="s">
-        <v>512</v>
+        <v>546</v>
       </c>
       <c r="G406" t="s">
         <v>28</v>
@@ -11429,11 +11484,11 @@
       <c r="B407" t="s">
         <v>702</v>
       </c>
-      <c r="C407" s="4" t="s">
-        <v>515</v>
+      <c r="C407" t="s">
+        <v>526</v>
       </c>
       <c r="D407" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G407" t="s">
         <v>28</v>
@@ -11446,11 +11501,11 @@
       <c r="B408" t="s">
         <v>702</v>
       </c>
-      <c r="C408" t="s">
-        <v>516</v>
+      <c r="C408" s="4" t="s">
+        <v>515</v>
       </c>
       <c r="D408" t="s">
-        <v>501</v>
+        <v>514</v>
       </c>
       <c r="G408" t="s">
         <v>28</v>
@@ -11464,10 +11519,13 @@
         <v>702</v>
       </c>
       <c r="C409" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D409" t="s">
-        <v>502</v>
+        <v>501</v>
+      </c>
+      <c r="G409" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.2">
@@ -11477,14 +11535,11 @@
       <c r="B410" t="s">
         <v>702</v>
       </c>
-      <c r="C410" s="4" t="s">
-        <v>538</v>
+      <c r="C410" t="s">
+        <v>517</v>
       </c>
       <c r="D410" t="s">
-        <v>918</v>
-      </c>
-      <c r="G410" t="s">
-        <v>28</v>
+        <v>502</v>
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.2">
@@ -11494,11 +11549,11 @@
       <c r="B411" t="s">
         <v>702</v>
       </c>
-      <c r="C411" t="s">
-        <v>539</v>
+      <c r="C411" s="4" t="s">
+        <v>538</v>
       </c>
       <c r="D411" t="s">
-        <v>531</v>
+        <v>918</v>
       </c>
       <c r="G411" t="s">
         <v>28</v>
@@ -11512,10 +11567,10 @@
         <v>702</v>
       </c>
       <c r="C412" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D412" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G412" t="s">
         <v>28</v>
@@ -11528,11 +11583,11 @@
       <c r="B413" t="s">
         <v>702</v>
       </c>
-      <c r="C413" s="4" t="s">
-        <v>522</v>
+      <c r="C413" t="s">
+        <v>541</v>
       </c>
       <c r="D413" t="s">
-        <v>507</v>
+        <v>532</v>
       </c>
       <c r="G413" t="s">
         <v>28</v>
@@ -11545,11 +11600,11 @@
       <c r="B414" t="s">
         <v>702</v>
       </c>
-      <c r="C414" t="s">
-        <v>523</v>
+      <c r="C414" s="4" t="s">
+        <v>522</v>
       </c>
       <c r="D414" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G414" t="s">
         <v>28</v>
@@ -11562,11 +11617,11 @@
       <c r="B415" t="s">
         <v>702</v>
       </c>
-      <c r="C415" s="4" t="s">
-        <v>524</v>
+      <c r="C415" t="s">
+        <v>523</v>
       </c>
       <c r="D415" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G415" t="s">
         <v>28</v>
@@ -11579,11 +11634,11 @@
       <c r="B416" t="s">
         <v>702</v>
       </c>
-      <c r="C416" s="12" t="s">
-        <v>525</v>
+      <c r="C416" s="4" t="s">
+        <v>524</v>
       </c>
       <c r="D416" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G416" t="s">
         <v>28</v>
@@ -11596,11 +11651,11 @@
       <c r="B417" t="s">
         <v>702</v>
       </c>
-      <c r="C417" t="s">
-        <v>689</v>
+      <c r="C417" s="12" t="s">
+        <v>525</v>
       </c>
       <c r="D417" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="G417" t="s">
         <v>28</v>
@@ -11613,11 +11668,14 @@
       <c r="B418" t="s">
         <v>702</v>
       </c>
-      <c r="C418" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="D418" s="53" t="s">
-        <v>667</v>
+      <c r="C418" t="s">
+        <v>689</v>
+      </c>
+      <c r="D418" t="s">
+        <v>503</v>
+      </c>
+      <c r="G418" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.2">
@@ -11628,10 +11686,10 @@
         <v>702</v>
       </c>
       <c r="C419" s="33" t="s">
-        <v>678</v>
+        <v>346</v>
       </c>
       <c r="D419" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.2">
@@ -11642,10 +11700,10 @@
         <v>702</v>
       </c>
       <c r="C420" s="33" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D420" s="53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="421" spans="1:7" x14ac:dyDescent="0.2">
@@ -11656,10 +11714,10 @@
         <v>702</v>
       </c>
       <c r="C421" s="33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D421" s="53" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.2">
@@ -11670,10 +11728,10 @@
         <v>702</v>
       </c>
       <c r="C422" s="33" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D422" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.2">
@@ -11684,10 +11742,10 @@
         <v>702</v>
       </c>
       <c r="C423" s="33" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="D423" s="53" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="424" spans="1:7" x14ac:dyDescent="0.2">
@@ -11698,10 +11756,10 @@
         <v>702</v>
       </c>
       <c r="C424" s="33" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D424" s="53" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="425" spans="1:7" x14ac:dyDescent="0.2">
@@ -11712,10 +11770,10 @@
         <v>702</v>
       </c>
       <c r="C425" s="33" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D425" s="53" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="426" spans="1:7" x14ac:dyDescent="0.2">
@@ -11726,10 +11784,10 @@
         <v>702</v>
       </c>
       <c r="C426" s="33" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D426" s="53" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="427" spans="1:7" x14ac:dyDescent="0.2">
@@ -11740,55 +11798,52 @@
         <v>702</v>
       </c>
       <c r="C427" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="D427" s="53" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>651</v>
+      </c>
+      <c r="B428" t="s">
+        <v>702</v>
+      </c>
+      <c r="C428" s="33" t="s">
         <v>685</v>
       </c>
-      <c r="D427" s="53" t="s">
+      <c r="D428" s="53" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A429" s="4" t="s">
+    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A430" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="B429" s="23" t="s">
+      <c r="B430" s="23" t="s">
         <v>914</v>
       </c>
-      <c r="C429" t="s">
+      <c r="C430" t="s">
         <v>60</v>
       </c>
-      <c r="D429" t="s">
+      <c r="D430" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A430" t="s">
-        <v>652</v>
-      </c>
-      <c r="B430" t="s">
-        <v>703</v>
-      </c>
-      <c r="C430" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="D430" t="s">
-        <v>500</v>
-      </c>
-      <c r="G430" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>687</v>
+        <v>652</v>
       </c>
       <c r="B431" t="s">
         <v>703</v>
       </c>
-      <c r="C431" t="s">
-        <v>516</v>
+      <c r="C431" s="4" t="s">
+        <v>515</v>
       </c>
       <c r="D431" t="s">
-        <v>542</v>
+        <v>500</v>
       </c>
       <c r="G431" t="s">
         <v>28</v>
@@ -11796,47 +11851,47 @@
     </row>
     <row r="432" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>652</v>
+        <v>687</v>
       </c>
       <c r="B432" t="s">
         <v>703</v>
       </c>
       <c r="C432" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D432" t="s">
-        <v>502</v>
+        <v>542</v>
+      </c>
+      <c r="G432" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="433" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>687</v>
+        <v>652</v>
       </c>
       <c r="B433" t="s">
         <v>703</v>
       </c>
-      <c r="C433" s="4" t="s">
-        <v>522</v>
+      <c r="C433" t="s">
+        <v>517</v>
       </c>
       <c r="D433" t="s">
-        <v>507</v>
-      </c>
-      <c r="G433" t="s">
-        <v>28</v>
+        <v>502</v>
       </c>
     </row>
     <row r="434" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>652</v>
+        <v>687</v>
       </c>
       <c r="B434" t="s">
         <v>703</v>
       </c>
-      <c r="C434" t="s">
-        <v>523</v>
+      <c r="C434" s="4" t="s">
+        <v>522</v>
       </c>
       <c r="D434" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G434" t="s">
         <v>28</v>
@@ -11849,11 +11904,11 @@
       <c r="B435" t="s">
         <v>703</v>
       </c>
-      <c r="C435" s="4" t="s">
-        <v>538</v>
+      <c r="C435" t="s">
+        <v>523</v>
       </c>
       <c r="D435" t="s">
-        <v>530</v>
+        <v>508</v>
       </c>
       <c r="G435" t="s">
         <v>28</v>
@@ -11866,11 +11921,11 @@
       <c r="B436" t="s">
         <v>703</v>
       </c>
-      <c r="C436" t="s">
-        <v>545</v>
+      <c r="C436" s="4" t="s">
+        <v>538</v>
       </c>
       <c r="D436" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="G436" t="s">
         <v>28</v>
@@ -11883,11 +11938,11 @@
       <c r="B437" t="s">
         <v>703</v>
       </c>
-      <c r="C437" s="4" t="s">
-        <v>536</v>
+      <c r="C437" t="s">
+        <v>545</v>
       </c>
       <c r="D437" t="s">
-        <v>527</v>
+        <v>543</v>
       </c>
       <c r="G437" t="s">
         <v>28</v>
@@ -11900,11 +11955,11 @@
       <c r="B438" t="s">
         <v>703</v>
       </c>
-      <c r="C438" t="s">
-        <v>537</v>
+      <c r="C438" s="4" t="s">
+        <v>536</v>
       </c>
       <c r="D438" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G438" t="s">
         <v>28</v>
@@ -11918,10 +11973,10 @@
         <v>703</v>
       </c>
       <c r="C439" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D439" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G439" t="s">
         <v>28</v>
@@ -11934,11 +11989,11 @@
       <c r="B440" t="s">
         <v>703</v>
       </c>
-      <c r="C440" s="4" t="s">
-        <v>459</v>
+      <c r="C440" t="s">
+        <v>540</v>
       </c>
       <c r="D440" t="s">
-        <v>450</v>
+        <v>529</v>
       </c>
       <c r="G440" t="s">
         <v>28</v>
@@ -11951,11 +12006,11 @@
       <c r="B441" t="s">
         <v>703</v>
       </c>
-      <c r="C441" t="s">
-        <v>495</v>
+      <c r="C441" s="4" t="s">
+        <v>459</v>
       </c>
       <c r="D441" t="s">
-        <v>544</v>
+        <v>450</v>
       </c>
       <c r="G441" t="s">
         <v>28</v>
@@ -11968,11 +12023,14 @@
       <c r="B442" t="s">
         <v>703</v>
       </c>
-      <c r="C442" s="33" t="s">
-        <v>917</v>
-      </c>
-      <c r="D442" s="53" t="s">
-        <v>667</v>
+      <c r="C442" t="s">
+        <v>495</v>
+      </c>
+      <c r="D442" t="s">
+        <v>544</v>
+      </c>
+      <c r="G442" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="443" spans="1:7" x14ac:dyDescent="0.2">
@@ -11983,10 +12041,10 @@
         <v>703</v>
       </c>
       <c r="C443" s="33" t="s">
-        <v>678</v>
+        <v>917</v>
       </c>
       <c r="D443" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="444" spans="1:7" x14ac:dyDescent="0.2">
@@ -11997,10 +12055,10 @@
         <v>703</v>
       </c>
       <c r="C444" s="33" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D444" s="53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.2">
@@ -12011,10 +12069,10 @@
         <v>703</v>
       </c>
       <c r="C445" s="33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D445" s="53" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.2">
@@ -12025,10 +12083,10 @@
         <v>703</v>
       </c>
       <c r="C446" s="33" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D446" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.2">
@@ -12039,10 +12097,10 @@
         <v>703</v>
       </c>
       <c r="C447" s="33" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="D447" s="53" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="448" spans="1:7" x14ac:dyDescent="0.2">
@@ -12053,10 +12111,10 @@
         <v>703</v>
       </c>
       <c r="C448" s="33" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D448" s="53" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="449" spans="1:7" x14ac:dyDescent="0.2">
@@ -12067,10 +12125,10 @@
         <v>703</v>
       </c>
       <c r="C449" s="33" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D449" s="53" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="450" spans="1:7" x14ac:dyDescent="0.2">
@@ -12081,10 +12139,10 @@
         <v>703</v>
       </c>
       <c r="C450" s="33" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D450" s="53" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="451" spans="1:7" x14ac:dyDescent="0.2">
@@ -12095,41 +12153,38 @@
         <v>703</v>
       </c>
       <c r="C451" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="D451" s="53" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A452" t="s">
+        <v>652</v>
+      </c>
+      <c r="B452" t="s">
+        <v>703</v>
+      </c>
+      <c r="C452" s="33" t="s">
         <v>685</v>
       </c>
-      <c r="D451" s="53" t="s">
+      <c r="D452" s="53" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A453" s="4" t="s">
+    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A454" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="B453" s="23" t="s">
+      <c r="B454" s="23" t="s">
         <v>915</v>
       </c>
-      <c r="C453" t="s">
+      <c r="C454" t="s">
         <v>60</v>
       </c>
-      <c r="D453" t="s">
+      <c r="D454" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A454" t="s">
-        <v>653</v>
-      </c>
-      <c r="B454" t="s">
-        <v>704</v>
-      </c>
-      <c r="C454" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="D454" t="s">
-        <v>557</v>
-      </c>
-      <c r="G454" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="455" spans="1:7" x14ac:dyDescent="0.2">
@@ -12140,10 +12195,13 @@
         <v>704</v>
       </c>
       <c r="C455" s="4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D455" t="s">
-        <v>559</v>
+        <v>557</v>
+      </c>
+      <c r="G455" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="456" spans="1:7" x14ac:dyDescent="0.2">
@@ -12154,10 +12212,10 @@
         <v>704</v>
       </c>
       <c r="C456" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D456" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
     </row>
     <row r="457" spans="1:7" x14ac:dyDescent="0.2">
@@ -12168,13 +12226,10 @@
         <v>704</v>
       </c>
       <c r="C457" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D457" t="s">
-        <v>562</v>
-      </c>
-      <c r="G457" t="s">
-        <v>28</v>
+        <v>548</v>
       </c>
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.2">
@@ -12184,11 +12239,11 @@
       <c r="B458" t="s">
         <v>704</v>
       </c>
-      <c r="C458" t="s">
-        <v>564</v>
+      <c r="C458" s="4" t="s">
+        <v>563</v>
       </c>
       <c r="D458" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="G458" t="s">
         <v>28</v>
@@ -12202,41 +12257,41 @@
         <v>704</v>
       </c>
       <c r="C459" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D459" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="G459" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="460" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A460" t="s">
+        <v>653</v>
+      </c>
       <c r="B460" t="s">
         <v>704</v>
       </c>
-      <c r="C460" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="D460" s="4" t="s">
-        <v>919</v>
+      <c r="C460" t="s">
+        <v>565</v>
+      </c>
+      <c r="D460" t="s">
+        <v>551</v>
+      </c>
+      <c r="G460" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="461" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A461" t="s">
-        <v>653</v>
-      </c>
       <c r="B461" t="s">
         <v>704</v>
       </c>
-      <c r="C461" t="s">
-        <v>566</v>
-      </c>
-      <c r="D461" t="s">
-        <v>550</v>
-      </c>
-      <c r="G461" t="s">
-        <v>28</v>
+      <c r="C461" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="D461" s="4" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="462" spans="1:7" x14ac:dyDescent="0.2">
@@ -12247,10 +12302,10 @@
         <v>704</v>
       </c>
       <c r="C462" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D462" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G462" t="s">
         <v>28</v>
@@ -12263,11 +12318,14 @@
       <c r="B463" t="s">
         <v>704</v>
       </c>
-      <c r="C463" s="4" t="s">
-        <v>578</v>
+      <c r="C463" t="s">
+        <v>567</v>
       </c>
       <c r="D463" t="s">
-        <v>553</v>
+        <v>552</v>
+      </c>
+      <c r="G463" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="464" spans="1:7" x14ac:dyDescent="0.2">
@@ -12278,13 +12336,10 @@
         <v>704</v>
       </c>
       <c r="C464" s="4" t="s">
-        <v>568</v>
+        <v>578</v>
       </c>
       <c r="D464" t="s">
-        <v>554</v>
-      </c>
-      <c r="G464" t="s">
-        <v>28</v>
+        <v>553</v>
       </c>
     </row>
     <row r="465" spans="1:7" x14ac:dyDescent="0.2">
@@ -12294,11 +12349,11 @@
       <c r="B465" t="s">
         <v>704</v>
       </c>
-      <c r="C465" t="s">
-        <v>569</v>
+      <c r="C465" s="4" t="s">
+        <v>568</v>
       </c>
       <c r="D465" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G465" t="s">
         <v>28</v>
@@ -12311,11 +12366,14 @@
       <c r="B466" t="s">
         <v>704</v>
       </c>
-      <c r="C466" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="D466" s="53" t="s">
-        <v>667</v>
+      <c r="C466" t="s">
+        <v>569</v>
+      </c>
+      <c r="D466" t="s">
+        <v>555</v>
+      </c>
+      <c r="G466" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.2">
@@ -12326,10 +12384,10 @@
         <v>704</v>
       </c>
       <c r="C467" s="33" t="s">
-        <v>678</v>
+        <v>346</v>
       </c>
       <c r="D467" s="53" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.2">
@@ -12340,10 +12398,10 @@
         <v>704</v>
       </c>
       <c r="C468" s="33" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D468" s="53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.2">
@@ -12354,10 +12412,10 @@
         <v>704</v>
       </c>
       <c r="C469" s="33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D469" s="53" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="470" spans="1:7" x14ac:dyDescent="0.2">
@@ -12368,10 +12426,10 @@
         <v>704</v>
       </c>
       <c r="C470" s="33" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D470" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="471" spans="1:7" x14ac:dyDescent="0.2">
@@ -12382,10 +12440,10 @@
         <v>704</v>
       </c>
       <c r="C471" s="33" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="D471" s="53" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="472" spans="1:7" x14ac:dyDescent="0.2">
@@ -12396,10 +12454,10 @@
         <v>704</v>
       </c>
       <c r="C472" s="33" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D472" s="53" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="473" spans="1:7" x14ac:dyDescent="0.2">
@@ -12410,10 +12468,10 @@
         <v>704</v>
       </c>
       <c r="C473" s="33" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D473" s="53" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="474" spans="1:7" x14ac:dyDescent="0.2">
@@ -12424,10 +12482,10 @@
         <v>704</v>
       </c>
       <c r="C474" s="33" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D474" s="53" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="475" spans="1:7" x14ac:dyDescent="0.2">
@@ -12438,41 +12496,38 @@
         <v>704</v>
       </c>
       <c r="C475" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="D475" s="53" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="476" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A476" t="s">
+        <v>653</v>
+      </c>
+      <c r="B476" t="s">
+        <v>704</v>
+      </c>
+      <c r="C476" s="33" t="s">
         <v>685</v>
       </c>
-      <c r="D475" s="53" t="s">
+      <c r="D476" s="53" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="477" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A477" s="4" t="s">
+    <row r="478" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A478" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="B477" s="23" t="s">
+      <c r="B478" s="23" t="s">
         <v>916</v>
       </c>
-      <c r="C477" t="s">
+      <c r="C478" t="s">
         <v>60</v>
       </c>
-      <c r="D477" t="s">
+      <c r="D478" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="478" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A478" t="s">
-        <v>654</v>
-      </c>
-      <c r="B478" t="s">
-        <v>705</v>
-      </c>
-      <c r="C478" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="D478" t="s">
-        <v>547</v>
-      </c>
-      <c r="G478" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="479" spans="1:7" x14ac:dyDescent="0.2">
@@ -12483,10 +12538,13 @@
         <v>705</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>920</v>
+        <v>558</v>
       </c>
       <c r="D479" t="s">
-        <v>570</v>
+        <v>547</v>
+      </c>
+      <c r="G479" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.2">
@@ -12497,10 +12555,10 @@
         <v>705</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D480" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="481" spans="1:7" x14ac:dyDescent="0.2">
@@ -12511,13 +12569,10 @@
         <v>705</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>576</v>
+        <v>921</v>
       </c>
       <c r="D481" t="s">
-        <v>575</v>
-      </c>
-      <c r="G481" t="s">
-        <v>28</v>
+        <v>571</v>
       </c>
     </row>
     <row r="482" spans="1:7" x14ac:dyDescent="0.2">
@@ -12528,10 +12583,13 @@
         <v>705</v>
       </c>
       <c r="C482" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D482" t="s">
-        <v>572</v>
+        <v>575</v>
+      </c>
+      <c r="G482" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="483" spans="1:7" x14ac:dyDescent="0.2">
@@ -12542,10 +12600,10 @@
         <v>705</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="D483" s="4" t="s">
-        <v>918</v>
+        <v>577</v>
+      </c>
+      <c r="D483" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="484" spans="1:7" x14ac:dyDescent="0.2">
@@ -12555,14 +12613,11 @@
       <c r="B484" t="s">
         <v>705</v>
       </c>
-      <c r="C484" t="s">
-        <v>545</v>
-      </c>
-      <c r="D484" t="s">
-        <v>543</v>
-      </c>
-      <c r="G484" t="s">
-        <v>28</v>
+      <c r="C484" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="D484" s="4" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="485" spans="1:7" x14ac:dyDescent="0.2">
@@ -12573,10 +12628,10 @@
         <v>705</v>
       </c>
       <c r="C485" t="s">
-        <v>581</v>
+        <v>545</v>
       </c>
       <c r="D485" t="s">
-        <v>573</v>
+        <v>543</v>
       </c>
       <c r="G485" t="s">
         <v>28</v>
@@ -12589,11 +12644,11 @@
       <c r="B486" t="s">
         <v>705</v>
       </c>
-      <c r="C486" s="4" t="s">
-        <v>563</v>
+      <c r="C486" t="s">
+        <v>581</v>
       </c>
       <c r="D486" t="s">
-        <v>549</v>
+        <v>573</v>
       </c>
       <c r="G486" t="s">
         <v>28</v>
@@ -12607,13 +12662,10 @@
         <v>705</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>580</v>
-      </c>
-      <c r="D487" t="s">
-        <v>579</v>
-      </c>
-      <c r="G487" t="s">
-        <v>28</v>
+        <v>931</v>
+      </c>
+      <c r="D487" s="16" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.2">
@@ -12623,14 +12675,11 @@
       <c r="B488" t="s">
         <v>705</v>
       </c>
-      <c r="C488" t="s">
-        <v>582</v>
-      </c>
-      <c r="D488" t="s">
-        <v>574</v>
-      </c>
-      <c r="G488" t="s">
-        <v>28</v>
+      <c r="C488" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="D488" s="16" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="489" spans="1:7" x14ac:dyDescent="0.2">
@@ -12641,10 +12690,10 @@
         <v>705</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>584</v>
+        <v>563</v>
       </c>
       <c r="D489" t="s">
-        <v>583</v>
+        <v>549</v>
       </c>
       <c r="G489" t="s">
         <v>28</v>
@@ -12657,11 +12706,14 @@
       <c r="B490" t="s">
         <v>705</v>
       </c>
-      <c r="C490" s="33" t="s">
-        <v>346</v>
-      </c>
-      <c r="D490" s="53" t="s">
-        <v>667</v>
+      <c r="C490" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="D490" t="s">
+        <v>579</v>
+      </c>
+      <c r="G490" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="491" spans="1:7" x14ac:dyDescent="0.2">
@@ -12671,11 +12723,14 @@
       <c r="B491" t="s">
         <v>705</v>
       </c>
-      <c r="C491" s="33" t="s">
-        <v>678</v>
-      </c>
-      <c r="D491" s="55" t="s">
-        <v>668</v>
+      <c r="C491" t="s">
+        <v>582</v>
+      </c>
+      <c r="D491" t="s">
+        <v>574</v>
+      </c>
+      <c r="G491" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="492" spans="1:7" x14ac:dyDescent="0.2">
@@ -12685,11 +12740,14 @@
       <c r="B492" t="s">
         <v>705</v>
       </c>
-      <c r="C492" s="33" t="s">
-        <v>679</v>
-      </c>
-      <c r="D492" s="56" t="s">
-        <v>669</v>
+      <c r="C492" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="D492" t="s">
+        <v>583</v>
+      </c>
+      <c r="G492" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="493" spans="1:7" x14ac:dyDescent="0.2">
@@ -12700,10 +12758,10 @@
         <v>705</v>
       </c>
       <c r="C493" s="33" t="s">
-        <v>680</v>
+        <v>346</v>
       </c>
       <c r="D493" s="53" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.2">
@@ -12714,10 +12772,10 @@
         <v>705</v>
       </c>
       <c r="C494" s="33" t="s">
-        <v>681</v>
-      </c>
-      <c r="D494" s="56" t="s">
-        <v>671</v>
+        <v>678</v>
+      </c>
+      <c r="D494" s="55" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="495" spans="1:7" x14ac:dyDescent="0.2">
@@ -12728,10 +12786,10 @@
         <v>705</v>
       </c>
       <c r="C495" s="33" t="s">
-        <v>677</v>
-      </c>
-      <c r="D495" s="53" t="s">
-        <v>672</v>
+        <v>679</v>
+      </c>
+      <c r="D495" s="56" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="496" spans="1:7" x14ac:dyDescent="0.2">
@@ -12742,10 +12800,10 @@
         <v>705</v>
       </c>
       <c r="C496" s="33" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D496" s="53" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.2">
@@ -12756,10 +12814,10 @@
         <v>705</v>
       </c>
       <c r="C497" s="33" t="s">
-        <v>683</v>
-      </c>
-      <c r="D497" s="53" t="s">
-        <v>674</v>
+        <v>681</v>
+      </c>
+      <c r="D497" s="56" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.2">
@@ -12770,10 +12828,10 @@
         <v>705</v>
       </c>
       <c r="C498" s="33" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="D498" s="53" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.2">
@@ -12784,52 +12842,52 @@
         <v>705</v>
       </c>
       <c r="C499" s="33" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D499" s="53" t="s">
-        <v>676</v>
+        <v>673</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>654</v>
+      </c>
+      <c r="B500" t="s">
+        <v>705</v>
+      </c>
+      <c r="C500" s="33" t="s">
+        <v>683</v>
+      </c>
+      <c r="D500" s="53" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
-        <v>122</v>
+        <v>654</v>
       </c>
       <c r="B501" t="s">
-        <v>706</v>
-      </c>
-      <c r="C501" s="8" t="s">
-        <v>612</v>
-      </c>
-      <c r="D501" t="s">
-        <v>611</v>
+        <v>705</v>
+      </c>
+      <c r="C501" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="D501" s="53" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
-        <v>122</v>
+        <v>654</v>
       </c>
       <c r="B502" t="s">
-        <v>706</v>
-      </c>
-      <c r="C502" t="s">
-        <v>123</v>
-      </c>
-      <c r="D502" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A503" t="s">
-        <v>122</v>
-      </c>
-      <c r="B503" t="s">
-        <v>706</v>
-      </c>
-      <c r="C503" t="s">
-        <v>125</v>
-      </c>
-      <c r="D503" t="s">
-        <v>126</v>
+        <v>705</v>
+      </c>
+      <c r="C502" s="33" t="s">
+        <v>685</v>
+      </c>
+      <c r="D502" s="53" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.2">
@@ -12839,11 +12897,11 @@
       <c r="B504" t="s">
         <v>706</v>
       </c>
-      <c r="C504" t="s">
-        <v>127</v>
+      <c r="C504" s="8" t="s">
+        <v>612</v>
       </c>
       <c r="D504" t="s">
-        <v>128</v>
+        <v>611</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.2">
@@ -12853,11 +12911,11 @@
       <c r="B505" t="s">
         <v>706</v>
       </c>
-      <c r="C505" s="8" t="s">
-        <v>129</v>
+      <c r="C505" t="s">
+        <v>123</v>
       </c>
       <c r="D505" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.2">
@@ -12868,10 +12926,10 @@
         <v>706</v>
       </c>
       <c r="C506" t="s">
-        <v>615</v>
+        <v>125</v>
       </c>
       <c r="D506" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.2">
@@ -12882,10 +12940,10 @@
         <v>706</v>
       </c>
       <c r="C507" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D507" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.2">
@@ -12895,11 +12953,11 @@
       <c r="B508" t="s">
         <v>706</v>
       </c>
-      <c r="C508" t="s">
-        <v>134</v>
+      <c r="C508" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="D508" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.2">
@@ -12910,10 +12968,10 @@
         <v>706</v>
       </c>
       <c r="C509" t="s">
-        <v>136</v>
+        <v>615</v>
       </c>
       <c r="D509" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.2">
@@ -12923,11 +12981,11 @@
       <c r="B510" t="s">
         <v>706</v>
       </c>
-      <c r="C510" s="8" t="s">
-        <v>138</v>
+      <c r="C510" t="s">
+        <v>132</v>
       </c>
       <c r="D510" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.2">
@@ -12938,10 +12996,10 @@
         <v>706</v>
       </c>
       <c r="C511" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D511" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.2">
@@ -12952,10 +13010,10 @@
         <v>706</v>
       </c>
       <c r="C512" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D512" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="513" spans="1:7" x14ac:dyDescent="0.2">
@@ -12965,11 +13023,11 @@
       <c r="B513" t="s">
         <v>706</v>
       </c>
-      <c r="C513" t="s">
-        <v>144</v>
+      <c r="C513" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="D513" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.2">
@@ -12980,13 +13038,10 @@
         <v>706</v>
       </c>
       <c r="C514" t="s">
-        <v>146</v>
-      </c>
-      <c r="D514" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G514" t="s">
-        <v>28</v>
+        <v>140</v>
+      </c>
+      <c r="D514" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="515" spans="1:7" x14ac:dyDescent="0.2">
@@ -12997,10 +13052,10 @@
         <v>706</v>
       </c>
       <c r="C515" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D515" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="516" spans="1:7" x14ac:dyDescent="0.2">
@@ -13011,10 +13066,10 @@
         <v>706</v>
       </c>
       <c r="C516" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D516" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="517" spans="1:7" x14ac:dyDescent="0.2">
@@ -13025,10 +13080,13 @@
         <v>706</v>
       </c>
       <c r="C517" t="s">
-        <v>152</v>
-      </c>
-      <c r="D517" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="D517" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G517" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.2">
@@ -13039,10 +13097,10 @@
         <v>706</v>
       </c>
       <c r="C518" t="s">
-        <v>613</v>
-      </c>
-      <c r="D518" s="15" t="s">
-        <v>614</v>
+        <v>148</v>
+      </c>
+      <c r="D518" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="519" spans="1:7" x14ac:dyDescent="0.2">
@@ -13053,10 +13111,10 @@
         <v>706</v>
       </c>
       <c r="C519" t="s">
-        <v>616</v>
-      </c>
-      <c r="D519" s="15" t="s">
-        <v>586</v>
+        <v>150</v>
+      </c>
+      <c r="D519" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="520" spans="1:7" x14ac:dyDescent="0.2">
@@ -13067,10 +13125,10 @@
         <v>706</v>
       </c>
       <c r="C520" t="s">
-        <v>617</v>
-      </c>
-      <c r="D520" s="15" t="s">
-        <v>587</v>
+        <v>152</v>
+      </c>
+      <c r="D520" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="521" spans="1:7" x14ac:dyDescent="0.2">
@@ -13081,10 +13139,10 @@
         <v>706</v>
       </c>
       <c r="C521" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D521" s="15" t="s">
-        <v>588</v>
+        <v>614</v>
       </c>
     </row>
     <row r="522" spans="1:7" x14ac:dyDescent="0.2">
@@ -13095,10 +13153,10 @@
         <v>706</v>
       </c>
       <c r="C522" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D522" s="15" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="523" spans="1:7" x14ac:dyDescent="0.2">
@@ -13109,10 +13167,10 @@
         <v>706</v>
       </c>
       <c r="C523" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D523" s="15" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="524" spans="1:7" x14ac:dyDescent="0.2">
@@ -13123,10 +13181,10 @@
         <v>706</v>
       </c>
       <c r="C524" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D524" s="15" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="525" spans="1:7" x14ac:dyDescent="0.2">
@@ -13137,10 +13195,10 @@
         <v>706</v>
       </c>
       <c r="C525" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D525" s="15" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="526" spans="1:7" x14ac:dyDescent="0.2">
@@ -13151,10 +13209,10 @@
         <v>706</v>
       </c>
       <c r="C526" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D526" s="15" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="527" spans="1:7" x14ac:dyDescent="0.2">
@@ -13165,10 +13223,10 @@
         <v>706</v>
       </c>
       <c r="C527" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D527" s="15" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.2">
@@ -13179,10 +13237,10 @@
         <v>706</v>
       </c>
       <c r="C528" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D528" s="15" t="s">
-        <v>626</v>
+        <v>592</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.2">
@@ -13193,10 +13251,10 @@
         <v>706</v>
       </c>
       <c r="C529" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D529" s="15" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.2">
@@ -13207,10 +13265,10 @@
         <v>706</v>
       </c>
       <c r="C530" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="D530" s="15" t="s">
-        <v>628</v>
+        <v>594</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.2">
@@ -13221,10 +13279,10 @@
         <v>706</v>
       </c>
       <c r="C531" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="D531" s="15" t="s">
-        <v>596</v>
+        <v>626</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.2">
@@ -13235,10 +13293,10 @@
         <v>706</v>
       </c>
       <c r="C532" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D532" s="15" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.2">
@@ -13249,10 +13307,10 @@
         <v>706</v>
       </c>
       <c r="C533" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D533" s="15" t="s">
-        <v>598</v>
+        <v>628</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.2">
@@ -13263,10 +13321,10 @@
         <v>706</v>
       </c>
       <c r="C534" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D534" s="15" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.2">
@@ -13277,10 +13335,10 @@
         <v>706</v>
       </c>
       <c r="C535" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D535" s="15" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.2">
@@ -13291,10 +13349,10 @@
         <v>706</v>
       </c>
       <c r="C536" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D536" s="15" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.2">
@@ -13305,10 +13363,10 @@
         <v>706</v>
       </c>
       <c r="C537" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D537" s="15" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.2">
@@ -13319,10 +13377,10 @@
         <v>706</v>
       </c>
       <c r="C538" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D538" s="15" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.2">
@@ -13333,10 +13391,10 @@
         <v>706</v>
       </c>
       <c r="C539" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D539" s="15" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.2">
@@ -13347,10 +13405,10 @@
         <v>706</v>
       </c>
       <c r="C540" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D540" s="15" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.2">
@@ -13361,10 +13419,10 @@
         <v>706</v>
       </c>
       <c r="C541" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D541" s="15" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.2">
@@ -13375,10 +13433,10 @@
         <v>706</v>
       </c>
       <c r="C542" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D542" s="15" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.2">
@@ -13389,10 +13447,10 @@
         <v>706</v>
       </c>
       <c r="C543" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D543" s="15" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.2">
@@ -13403,10 +13461,10 @@
         <v>706</v>
       </c>
       <c r="C544" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D544" s="15" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.2">
@@ -13417,52 +13475,52 @@
         <v>706</v>
       </c>
       <c r="C545" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D545" s="15" t="s">
-        <v>610</v>
+        <v>607</v>
+      </c>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A546" t="s">
+        <v>122</v>
+      </c>
+      <c r="B546" t="s">
+        <v>706</v>
+      </c>
+      <c r="C546" t="s">
+        <v>642</v>
+      </c>
+      <c r="D546" s="15" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B547" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C547" t="s">
-        <v>154</v>
-      </c>
-      <c r="D547" t="s">
-        <v>155</v>
+        <v>643</v>
+      </c>
+      <c r="D547" s="15" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B548" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C548" t="s">
-        <v>157</v>
-      </c>
-      <c r="D548" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="549" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A549" t="s">
-        <v>156</v>
-      </c>
-      <c r="B549" t="s">
-        <v>707</v>
-      </c>
-      <c r="C549" t="s">
-        <v>159</v>
-      </c>
-      <c r="D549" t="s">
-        <v>160</v>
+        <v>644</v>
+      </c>
+      <c r="D548" s="15" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.2">
@@ -13473,10 +13531,10 @@
         <v>707</v>
       </c>
       <c r="C550" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D550" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.2">
@@ -13486,14 +13544,11 @@
       <c r="B551" t="s">
         <v>707</v>
       </c>
-      <c r="C551" s="8" t="s">
-        <v>163</v>
+      <c r="C551" t="s">
+        <v>157</v>
       </c>
       <c r="D551" t="s">
-        <v>164</v>
-      </c>
-      <c r="G551" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
     </row>
     <row r="552" spans="1:7" x14ac:dyDescent="0.2">
@@ -13504,10 +13559,10 @@
         <v>707</v>
       </c>
       <c r="C552" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D552" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.2">
@@ -13518,10 +13573,10 @@
         <v>707</v>
       </c>
       <c r="C553" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D553" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.2">
@@ -13531,11 +13586,14 @@
       <c r="B554" t="s">
         <v>707</v>
       </c>
-      <c r="C554" t="s">
-        <v>169</v>
+      <c r="C554" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="D554" t="s">
-        <v>170</v>
+        <v>164</v>
+      </c>
+      <c r="G554" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.2">
@@ -13545,14 +13603,11 @@
       <c r="B555" t="s">
         <v>707</v>
       </c>
-      <c r="C555" s="8" t="s">
-        <v>171</v>
+      <c r="C555" t="s">
+        <v>165</v>
       </c>
       <c r="D555" t="s">
-        <v>172</v>
-      </c>
-      <c r="G555" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.2">
@@ -13563,10 +13618,10 @@
         <v>707</v>
       </c>
       <c r="C556" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D556" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.2">
@@ -13577,10 +13632,10 @@
         <v>707</v>
       </c>
       <c r="C557" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D557" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.2">
@@ -13590,11 +13645,14 @@
       <c r="B558" t="s">
         <v>707</v>
       </c>
-      <c r="C558" t="s">
-        <v>177</v>
+      <c r="C558" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="D558" t="s">
-        <v>178</v>
+        <v>172</v>
+      </c>
+      <c r="G558" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="559" spans="1:7" x14ac:dyDescent="0.2">
@@ -13604,14 +13662,11 @@
       <c r="B559" t="s">
         <v>707</v>
       </c>
-      <c r="C559" s="8" t="s">
-        <v>179</v>
+      <c r="C559" t="s">
+        <v>173</v>
       </c>
       <c r="D559" t="s">
-        <v>180</v>
-      </c>
-      <c r="G559" t="s">
-        <v>28</v>
+        <v>174</v>
       </c>
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.2">
@@ -13622,10 +13677,10 @@
         <v>707</v>
       </c>
       <c r="C560" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D560" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.2">
@@ -13635,14 +13690,11 @@
       <c r="B561" t="s">
         <v>707</v>
       </c>
-      <c r="C561" s="8" t="s">
-        <v>183</v>
+      <c r="C561" t="s">
+        <v>177</v>
       </c>
       <c r="D561" t="s">
-        <v>184</v>
-      </c>
-      <c r="G561" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
     </row>
     <row r="562" spans="1:7" x14ac:dyDescent="0.2">
@@ -13652,11 +13704,14 @@
       <c r="B562" t="s">
         <v>707</v>
       </c>
-      <c r="C562" t="s">
-        <v>185</v>
+      <c r="C562" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="D562" t="s">
-        <v>186</v>
+        <v>180</v>
+      </c>
+      <c r="G562" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.2">
@@ -13666,14 +13721,11 @@
       <c r="B563" t="s">
         <v>707</v>
       </c>
-      <c r="C563" s="8" t="s">
-        <v>187</v>
+      <c r="C563" t="s">
+        <v>181</v>
       </c>
       <c r="D563" t="s">
-        <v>188</v>
-      </c>
-      <c r="G563" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
     </row>
     <row r="564" spans="1:7" x14ac:dyDescent="0.2">
@@ -13683,11 +13735,14 @@
       <c r="B564" t="s">
         <v>707</v>
       </c>
-      <c r="C564" t="s">
-        <v>189</v>
+      <c r="C564" s="8" t="s">
+        <v>183</v>
       </c>
       <c r="D564" t="s">
-        <v>341</v>
+        <v>184</v>
+      </c>
+      <c r="G564" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="565" spans="1:7" x14ac:dyDescent="0.2">
@@ -13698,13 +13753,10 @@
         <v>707</v>
       </c>
       <c r="C565" t="s">
-        <v>340</v>
-      </c>
-      <c r="D565" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="G565" t="s">
-        <v>28</v>
+        <v>185</v>
+      </c>
+      <c r="D565" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="566" spans="1:7" x14ac:dyDescent="0.2">
@@ -13714,11 +13766,14 @@
       <c r="B566" t="s">
         <v>707</v>
       </c>
-      <c r="C566" t="s">
-        <v>190</v>
+      <c r="C566" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="D566" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="G566" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="567" spans="1:7" x14ac:dyDescent="0.2">
@@ -13729,10 +13784,10 @@
         <v>707</v>
       </c>
       <c r="C567" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D567" t="s">
-        <v>193</v>
+        <v>341</v>
       </c>
     </row>
     <row r="568" spans="1:7" x14ac:dyDescent="0.2">
@@ -13743,10 +13798,13 @@
         <v>707</v>
       </c>
       <c r="C568" t="s">
-        <v>194</v>
-      </c>
-      <c r="D568" t="s">
-        <v>195</v>
+        <v>340</v>
+      </c>
+      <c r="D568" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G568" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.2">
@@ -13757,10 +13815,10 @@
         <v>707</v>
       </c>
       <c r="C569" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D569" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.2">
@@ -13771,10 +13829,10 @@
         <v>707</v>
       </c>
       <c r="C570" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D570" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.2">
@@ -13785,10 +13843,10 @@
         <v>707</v>
       </c>
       <c r="C571" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D571" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.2">
@@ -13799,10 +13857,10 @@
         <v>707</v>
       </c>
       <c r="C572" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D572" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.2">
@@ -13813,10 +13871,10 @@
         <v>707</v>
       </c>
       <c r="C573" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D573" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.2">
@@ -13827,10 +13885,10 @@
         <v>707</v>
       </c>
       <c r="C574" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D574" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.2">
@@ -13841,72 +13899,66 @@
         <v>707</v>
       </c>
       <c r="C575" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D575" t="s">
-        <v>209</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A576" t="s">
+        <v>156</v>
+      </c>
+      <c r="B576" t="s">
+        <v>707</v>
+      </c>
+      <c r="C576" t="s">
+        <v>204</v>
+      </c>
+      <c r="D576" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A577" s="4" t="s">
-        <v>718</v>
-      </c>
-      <c r="B577" s="4" t="s">
-        <v>708</v>
+      <c r="A577" t="s">
+        <v>156</v>
+      </c>
+      <c r="B577" t="s">
+        <v>707</v>
       </c>
       <c r="C577" t="s">
-        <v>88</v>
+        <v>206</v>
       </c>
       <c r="D577" t="s">
-        <v>94</v>
+        <v>207</v>
       </c>
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>212</v>
+        <v>156</v>
       </c>
       <c r="B578" t="s">
+        <v>707</v>
+      </c>
+      <c r="C578" t="s">
+        <v>208</v>
+      </c>
+      <c r="D578" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A580" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="B580" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="C578" t="s">
-        <v>210</v>
-      </c>
-      <c r="D578" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G578" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="579" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A579" t="s">
-        <v>212</v>
-      </c>
-      <c r="B579" t="s">
-        <v>708</v>
-      </c>
-      <c r="C579" t="s">
-        <v>213</v>
-      </c>
-      <c r="D579" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G579" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="580" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A580" t="s">
-        <v>212</v>
-      </c>
-      <c r="B580" t="s">
-        <v>708</v>
-      </c>
       <c r="C580" t="s">
-        <v>215</v>
+        <v>88</v>
       </c>
       <c r="D580" t="s">
-        <v>216</v>
+        <v>94</v>
       </c>
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.2">
@@ -13917,10 +13969,13 @@
         <v>708</v>
       </c>
       <c r="C581" t="s">
-        <v>217</v>
-      </c>
-      <c r="D581" t="s">
-        <v>218</v>
+        <v>210</v>
+      </c>
+      <c r="D581" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G581" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.2">
@@ -13930,11 +13985,11 @@
       <c r="B582" t="s">
         <v>708</v>
       </c>
-      <c r="C582" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="D582" s="2" t="s">
-        <v>220</v>
+      <c r="C582" t="s">
+        <v>213</v>
+      </c>
+      <c r="D582" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="G582" t="s">
         <v>28</v>
@@ -13948,10 +14003,10 @@
         <v>708</v>
       </c>
       <c r="C583" t="s">
-        <v>221</v>
-      </c>
-      <c r="D583" s="2" t="s">
-        <v>222</v>
+        <v>215</v>
+      </c>
+      <c r="D583" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.2">
@@ -13962,10 +14017,10 @@
         <v>708</v>
       </c>
       <c r="C584" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D584" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.2">
@@ -13975,11 +14030,11 @@
       <c r="B585" t="s">
         <v>708</v>
       </c>
-      <c r="C585" t="s">
-        <v>225</v>
-      </c>
-      <c r="D585" s="3" t="s">
-        <v>226</v>
+      <c r="C585" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D585" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="G585" t="s">
         <v>28</v>
@@ -13993,10 +14048,10 @@
         <v>708</v>
       </c>
       <c r="C586" t="s">
-        <v>227</v>
-      </c>
-      <c r="D586" t="s">
-        <v>228</v>
+        <v>221</v>
+      </c>
+      <c r="D586" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.2">
@@ -14007,10 +14062,10 @@
         <v>708</v>
       </c>
       <c r="C587" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D587" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.2">
@@ -14021,10 +14076,13 @@
         <v>708</v>
       </c>
       <c r="C588" t="s">
-        <v>231</v>
-      </c>
-      <c r="D588" t="s">
-        <v>232</v>
+        <v>225</v>
+      </c>
+      <c r="D588" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G588" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.2">
@@ -14035,10 +14093,10 @@
         <v>708</v>
       </c>
       <c r="C589" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D589" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.2">
@@ -14049,10 +14107,10 @@
         <v>708</v>
       </c>
       <c r="C590" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D590" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.2">
@@ -14063,10 +14121,10 @@
         <v>708</v>
       </c>
       <c r="C591" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D591" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.2">
@@ -14077,10 +14135,10 @@
         <v>708</v>
       </c>
       <c r="C592" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D592" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.2">
@@ -14091,10 +14149,10 @@
         <v>708</v>
       </c>
       <c r="C593" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D593" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.2">
@@ -14105,13 +14163,10 @@
         <v>708</v>
       </c>
       <c r="C594" t="s">
-        <v>243</v>
-      </c>
-      <c r="D594" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="G594" t="s">
-        <v>28</v>
+        <v>237</v>
+      </c>
+      <c r="D594" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.2">
@@ -14122,13 +14177,10 @@
         <v>708</v>
       </c>
       <c r="C595" t="s">
-        <v>245</v>
-      </c>
-      <c r="D595" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G595" t="s">
-        <v>28</v>
+        <v>239</v>
+      </c>
+      <c r="D595" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.2">
@@ -14139,10 +14191,10 @@
         <v>708</v>
       </c>
       <c r="C596" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D596" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.2">
@@ -14153,10 +14205,13 @@
         <v>708</v>
       </c>
       <c r="C597" t="s">
-        <v>249</v>
-      </c>
-      <c r="D597" t="s">
-        <v>250</v>
+        <v>243</v>
+      </c>
+      <c r="D597" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G597" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="598" spans="1:7" x14ac:dyDescent="0.2">
@@ -14167,10 +14222,10 @@
         <v>708</v>
       </c>
       <c r="C598" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D598" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G598" t="s">
         <v>28</v>
@@ -14184,13 +14239,10 @@
         <v>708</v>
       </c>
       <c r="C599" t="s">
-        <v>253</v>
-      </c>
-      <c r="D599" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="G599" t="s">
-        <v>28</v>
+        <v>247</v>
+      </c>
+      <c r="D599" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.2">
@@ -14201,10 +14253,10 @@
         <v>708</v>
       </c>
       <c r="C600" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D600" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.2">
@@ -14215,10 +14267,13 @@
         <v>708</v>
       </c>
       <c r="C601" t="s">
-        <v>257</v>
-      </c>
-      <c r="D601" t="s">
-        <v>258</v>
+        <v>251</v>
+      </c>
+      <c r="D601" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G601" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.2">
@@ -14229,10 +14284,13 @@
         <v>708</v>
       </c>
       <c r="C602" t="s">
-        <v>259</v>
-      </c>
-      <c r="D602" t="s">
-        <v>260</v>
+        <v>253</v>
+      </c>
+      <c r="D602" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G602" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="603" spans="1:7" x14ac:dyDescent="0.2">
@@ -14243,66 +14301,66 @@
         <v>708</v>
       </c>
       <c r="C603" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D603" t="s">
-        <v>262</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A604" t="s">
+        <v>212</v>
+      </c>
+      <c r="B604" t="s">
+        <v>708</v>
+      </c>
+      <c r="C604" t="s">
+        <v>257</v>
+      </c>
+      <c r="D604" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A605" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B605" s="4" t="s">
-        <v>709</v>
+      <c r="A605" t="s">
+        <v>212</v>
+      </c>
+      <c r="B605" t="s">
+        <v>708</v>
       </c>
       <c r="C605" t="s">
-        <v>88</v>
+        <v>259</v>
       </c>
       <c r="D605" t="s">
-        <v>94</v>
+        <v>260</v>
       </c>
     </row>
     <row r="606" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
+        <v>212</v>
+      </c>
+      <c r="B606" t="s">
+        <v>708</v>
+      </c>
+      <c r="C606" t="s">
+        <v>261</v>
+      </c>
+      <c r="D606" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="608" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A608" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B606" t="s">
+      <c r="B608" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="C606" t="s">
-        <v>263</v>
-      </c>
-      <c r="D606" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="607" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A607" t="s">
-        <v>265</v>
-      </c>
-      <c r="B607" t="s">
-        <v>709</v>
-      </c>
-      <c r="C607" t="s">
-        <v>266</v>
-      </c>
-      <c r="D607" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="608" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A608" t="s">
-        <v>265</v>
-      </c>
-      <c r="B608" t="s">
-        <v>709</v>
-      </c>
       <c r="C608" t="s">
-        <v>268</v>
+        <v>88</v>
       </c>
       <c r="D608" t="s">
-        <v>269</v>
+        <v>94</v>
       </c>
     </row>
     <row r="609" spans="1:4" x14ac:dyDescent="0.2">
@@ -14313,10 +14371,10 @@
         <v>709</v>
       </c>
       <c r="C609" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D609" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="610" spans="1:4" x14ac:dyDescent="0.2">
@@ -14327,10 +14385,10 @@
         <v>709</v>
       </c>
       <c r="C610" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D610" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="611" spans="1:4" x14ac:dyDescent="0.2">
@@ -14341,10 +14399,10 @@
         <v>709</v>
       </c>
       <c r="C611" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D611" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="612" spans="1:4" x14ac:dyDescent="0.2">
@@ -14355,10 +14413,10 @@
         <v>709</v>
       </c>
       <c r="C612" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D612" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="613" spans="1:4" x14ac:dyDescent="0.2">
@@ -14369,10 +14427,10 @@
         <v>709</v>
       </c>
       <c r="C613" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D613" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="614" spans="1:4" x14ac:dyDescent="0.2">
@@ -14383,10 +14441,10 @@
         <v>709</v>
       </c>
       <c r="C614" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D614" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="615" spans="1:4" x14ac:dyDescent="0.2">
@@ -14397,10 +14455,10 @@
         <v>709</v>
       </c>
       <c r="C615" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D615" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="616" spans="1:4" x14ac:dyDescent="0.2">
@@ -14411,10 +14469,10 @@
         <v>709</v>
       </c>
       <c r="C616" t="s">
-        <v>243</v>
+        <v>278</v>
       </c>
       <c r="D616" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="617" spans="1:4" x14ac:dyDescent="0.2">
@@ -14425,10 +14483,10 @@
         <v>709</v>
       </c>
       <c r="C617" t="s">
-        <v>245</v>
+        <v>280</v>
       </c>
       <c r="D617" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.2">
@@ -14439,10 +14497,10 @@
         <v>709</v>
       </c>
       <c r="C618" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D618" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="619" spans="1:4" x14ac:dyDescent="0.2">
@@ -14453,10 +14511,10 @@
         <v>709</v>
       </c>
       <c r="C619" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D619" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="620" spans="1:4" x14ac:dyDescent="0.2">
@@ -14467,66 +14525,66 @@
         <v>709</v>
       </c>
       <c r="C620" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D620" t="s">
-        <v>289</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A621" t="s">
+        <v>265</v>
+      </c>
+      <c r="B621" t="s">
+        <v>709</v>
+      </c>
+      <c r="C621" t="s">
+        <v>286</v>
+      </c>
+      <c r="D621" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A622" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="B622" s="4" t="s">
-        <v>710</v>
+      <c r="A622" t="s">
+        <v>265</v>
+      </c>
+      <c r="B622" t="s">
+        <v>709</v>
       </c>
       <c r="C622" t="s">
-        <v>88</v>
+        <v>249</v>
       </c>
       <c r="D622" t="s">
-        <v>94</v>
+        <v>288</v>
       </c>
     </row>
     <row r="623" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
+        <v>265</v>
+      </c>
+      <c r="B623" t="s">
+        <v>709</v>
+      </c>
+      <c r="C623" t="s">
+        <v>247</v>
+      </c>
+      <c r="D623" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A625" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="B623" t="s">
+      <c r="B625" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="C623" t="s">
-        <v>290</v>
-      </c>
-      <c r="D623" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="624" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A624" t="s">
-        <v>292</v>
-      </c>
-      <c r="B624" t="s">
-        <v>710</v>
-      </c>
-      <c r="C624" t="s">
-        <v>293</v>
-      </c>
-      <c r="D624" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A625" t="s">
-        <v>292</v>
-      </c>
-      <c r="B625" t="s">
-        <v>710</v>
-      </c>
       <c r="C625" t="s">
-        <v>295</v>
+        <v>88</v>
       </c>
       <c r="D625" t="s">
-        <v>296</v>
+        <v>94</v>
       </c>
     </row>
     <row r="626" spans="1:4" x14ac:dyDescent="0.2">
@@ -14537,10 +14595,10 @@
         <v>710</v>
       </c>
       <c r="C626" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D626" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="627" spans="1:4" x14ac:dyDescent="0.2">
@@ -14551,10 +14609,10 @@
         <v>710</v>
       </c>
       <c r="C627" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D627" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="628" spans="1:4" x14ac:dyDescent="0.2">
@@ -14564,11 +14622,11 @@
       <c r="B628" t="s">
         <v>710</v>
       </c>
-      <c r="C628" s="8" t="s">
-        <v>301</v>
+      <c r="C628" t="s">
+        <v>295</v>
       </c>
       <c r="D628" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="629" spans="1:4" x14ac:dyDescent="0.2">
@@ -14579,10 +14637,10 @@
         <v>710</v>
       </c>
       <c r="C629" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D629" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="630" spans="1:4" x14ac:dyDescent="0.2">
@@ -14593,10 +14651,10 @@
         <v>710</v>
       </c>
       <c r="C630" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D630" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="631" spans="1:4" x14ac:dyDescent="0.2">
@@ -14606,11 +14664,11 @@
       <c r="B631" t="s">
         <v>710</v>
       </c>
-      <c r="C631" t="s">
-        <v>307</v>
+      <c r="C631" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="D631" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.2">
@@ -14621,10 +14679,10 @@
         <v>710</v>
       </c>
       <c r="C632" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D632" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="633" spans="1:4" x14ac:dyDescent="0.2">
@@ -14634,11 +14692,11 @@
       <c r="B633" t="s">
         <v>710</v>
       </c>
-      <c r="C633" s="8" t="s">
-        <v>311</v>
+      <c r="C633" t="s">
+        <v>305</v>
       </c>
       <c r="D633" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="634" spans="1:4" x14ac:dyDescent="0.2">
@@ -14649,10 +14707,10 @@
         <v>710</v>
       </c>
       <c r="C634" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D634" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="635" spans="1:4" x14ac:dyDescent="0.2">
@@ -14663,10 +14721,10 @@
         <v>710</v>
       </c>
       <c r="C635" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D635" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="636" spans="1:4" x14ac:dyDescent="0.2">
@@ -14676,11 +14734,11 @@
       <c r="B636" t="s">
         <v>710</v>
       </c>
-      <c r="C636" t="s">
-        <v>317</v>
+      <c r="C636" s="8" t="s">
+        <v>311</v>
       </c>
       <c r="D636" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="637" spans="1:4" x14ac:dyDescent="0.2">
@@ -14691,10 +14749,10 @@
         <v>710</v>
       </c>
       <c r="C637" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D637" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="638" spans="1:4" x14ac:dyDescent="0.2">
@@ -14705,10 +14763,10 @@
         <v>710</v>
       </c>
       <c r="C638" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D638" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="639" spans="1:4" x14ac:dyDescent="0.2">
@@ -14719,10 +14777,10 @@
         <v>710</v>
       </c>
       <c r="C639" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D639" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="640" spans="1:4" x14ac:dyDescent="0.2">
@@ -14733,10 +14791,10 @@
         <v>710</v>
       </c>
       <c r="C640" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D640" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.2">
@@ -14747,10 +14805,10 @@
         <v>710</v>
       </c>
       <c r="C641" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D641" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.2">
@@ -14760,11 +14818,11 @@
       <c r="B642" t="s">
         <v>710</v>
       </c>
-      <c r="C642" s="8" t="s">
-        <v>144</v>
+      <c r="C642" t="s">
+        <v>323</v>
       </c>
       <c r="D642" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.2">
@@ -14775,10 +14833,10 @@
         <v>710</v>
       </c>
       <c r="C643" t="s">
-        <v>146</v>
+        <v>325</v>
       </c>
       <c r="D643" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.2">
@@ -14789,10 +14847,10 @@
         <v>710</v>
       </c>
       <c r="C644" t="s">
-        <v>148</v>
+        <v>327</v>
       </c>
       <c r="D644" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.2">
@@ -14802,11 +14860,11 @@
       <c r="B645" t="s">
         <v>710</v>
       </c>
-      <c r="C645" t="s">
-        <v>332</v>
+      <c r="C645" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="D645" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.2">
@@ -14817,10 +14875,10 @@
         <v>710</v>
       </c>
       <c r="C646" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D646" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.2">
@@ -14831,12 +14889,54 @@
         <v>710</v>
       </c>
       <c r="C647" t="s">
+        <v>148</v>
+      </c>
+      <c r="D647" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="648" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A648" t="s">
+        <v>292</v>
+      </c>
+      <c r="B648" t="s">
+        <v>710</v>
+      </c>
+      <c r="C648" t="s">
+        <v>332</v>
+      </c>
+      <c r="D648" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="649" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A649" t="s">
+        <v>292</v>
+      </c>
+      <c r="B649" t="s">
+        <v>710</v>
+      </c>
+      <c r="C649" t="s">
+        <v>152</v>
+      </c>
+      <c r="D649" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="650" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A650" t="s">
+        <v>292</v>
+      </c>
+      <c r="B650" t="s">
+        <v>710</v>
+      </c>
+      <c r="C650" t="s">
         <v>335</v>
       </c>
-      <c r="D647" s="3" t="s">
+      <c r="D650" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="G647" t="s">
+      <c r="G650" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>